<commit_message>
Avances en funcionalidad de plantillas de Proyecto
</commit_message>
<xml_diff>
--- a/docs/trim01/04_requisitos_funcionales_y_no_funcionales/REQUISITOS FUNCIONALES PROYECTO.xlsx
+++ b/docs/trim01/04_requisitos_funcionales_y_no_funcionales/REQUISITOS FUNCIONALES PROYECTO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7eb5a46966f243cc/Documentos/ANALISIS Y DESARROLLO DE SOFTWARE (2919581)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_9DA62F1B8F2B3910446563EAD332B0D17AC39BE9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF45EAD9-181C-4FF0-814D-CAA78319D921}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_9DA62F1B8F2B3910446563EAD332B0D17AC39BE9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03D99FCA-162B-4973-8275-63186BB2B0AE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REQUISITOS_MODULO_USUARIOS" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="146">
   <si>
     <t>MODULO</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Editar Proyecto</t>
   </si>
   <si>
-    <t>El sistema debe permitir al Administrador, Lider de proyecto y Miembro de Proyecto Editar Proyecto</t>
-  </si>
-  <si>
     <t>Eliminar Proyecto</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
   </si>
   <si>
     <t>Filtrar Proyecto</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir al Administrador, Lider de poyecto y Miembro de proyecto Filtrar Proyecto</t>
   </si>
   <si>
     <t xml:space="preserve">Gestionar Permisos </t>
@@ -472,6 +466,18 @@
   </si>
   <si>
     <t>El sistema debe permitir al Administrador, Lider de proyecto, Miembro de proyecto y cliente/StakeHolder Modificar su Contraseña en la edición de su perfil</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al Administrador, Lider de proyecto Editar Proyecto</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al Administrador, Lider de poyecto, Miembro de proyecto y cliente/StakeHolder Filtrar Proyecto</t>
+  </si>
+  <si>
+    <t>Eliminar Plantillas de Proyecto</t>
+  </si>
+  <si>
+    <t>El sistema deberá permitir al Administrador y Lider de proyecto Eliminar Plantillas de Proyecto</t>
   </si>
 </sst>
 </file>
@@ -815,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -901,7 +907,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -915,10 +921,10 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" t="s">
         <v>141</v>
-      </c>
-      <c r="C7" t="s">
-        <v>143</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1133,7 +1139,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
         <v>57</v>
@@ -1156,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1258,16 +1264,16 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1275,10 +1281,10 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1292,10 +1298,10 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -1309,10 +1315,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1326,10 +1332,10 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1343,10 +1349,10 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -1360,10 +1366,10 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -1377,10 +1383,10 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -1394,10 +1400,10 @@
         <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -1411,10 +1417,10 @@
         <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -1428,10 +1434,10 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -1440,7 +1446,25 @@
         <v>13</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1467,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -1498,10 +1522,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -1518,7 +1542,7 @@
         <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1549,10 +1573,10 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1566,10 +1590,10 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1583,10 +1607,10 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -1600,10 +1624,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1617,10 +1641,10 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1634,10 +1658,10 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -1673,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -1704,10 +1728,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -1721,10 +1745,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1738,10 +1762,10 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1755,10 +1779,10 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1772,10 +1796,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -1789,10 +1813,10 @@
         <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -1806,10 +1830,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1823,10 +1847,10 @@
         <v>31</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1840,10 +1864,10 @@
         <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -1879,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -1910,10 +1934,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -1927,10 +1951,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1944,10 +1968,10 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1961,10 +1985,10 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1978,10 +2002,10 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1995,10 +2019,10 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -2012,10 +2036,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -2029,10 +2053,10 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>

</xml_diff>